<commit_message>
New translations extracted_bad_strings.xlsx (French)
</commit_message>
<xml_diff>
--- a/fr/extracted_bad_strings.xlsx
+++ b/fr/extracted_bad_strings.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="134">
   <si>
     <t>Texte Japonais</t>
   </si>
@@ -33,11 +33,48 @@
 &lt;case_end&gt;</t>
   </si>
   <si>
+    <t xml:space="preserve">&lt;attr&gt;&lt;feel_normal_one&gt;&lt;end_attr&gt;You've returned! I assume that means you've
+successfully completed your initiation exam,
+right?!
+&lt;select&gt;
+Yes sir!
+No, sir.
+&lt;select_end&gt;
+&lt;case 1&gt;
+&lt;break&gt;
+&lt;case 2&gt;
+&lt;break&gt;
+&lt;case_cancel&gt;
+&lt;break&gt;
+&lt;case_end&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;attr&gt;&lt;feel_normal_one&gt;&lt;end_attr&gt;Tu as bien passe l’epreuve d’entree, hein?!
+&lt;select&gt;
+Oui, chef!
+Non.
+&lt;select_end&gt;
+&lt;case 1&gt;
+&lt;break&gt;
+&lt;case 2&gt;
+&lt;break&gt;
+&lt;case_cancel&gt;
+&lt;break&gt;
+&lt;case_end&gt;</t>
+  </si>
+  <si>
     <t>解放の扉に到達した！</t>
+  </si>
+  <si>
+    <t>You've reached the Door of Return!</t>
   </si>
   <si>
     <t xml:space="preserve">階に移動できそうだ。
 移動しますか？&lt;yesno&gt;&lt;close&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You can proceed to the next floor down from
+here. Go to the next floor?&lt;yesno&gt;&lt;close&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">はじめての町に　着きました！
@@ -45,13 +82,33 @@
 </t>
   </si>
   <si>
+    <t xml:space="preserve">This is your first visit to this town! It may
+be advantageous to change your resurrection
+spot to here in case your party is defeated.
+&lt;br&gt;
+Change your current resurrection spot to
+this town?&lt;yesno 2&gt;&lt;break&gt;</t>
+  </si>
+  <si>
     <t xml:space="preserve">　すべてのスキルで
 スキルポイントを　２０Ｐかくとく！
 &lt;color_yellow&gt;スキルふりわけ画面で　確認しましょう。 &lt;color_white&gt;&lt;me 71&gt;&lt;bw_break&gt;</t>
   </si>
   <si>
+    <t xml:space="preserve">Received 20 skill points in all of your skill
+lines!
+&lt;color_yellow&gt;Check the "Skill Points" screen.&lt;color_white&gt;&lt;me 71&gt;&lt;bw_break&gt;</t>
+  </si>
+  <si>
     <t xml:space="preserve">冒険者のあなたに　心強い仲間と
 すぐに　強くなれる帽子を　用意しました。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Welcome to Astoltia!
+&lt;br&gt;
+As an adventurer beginning past Version 1,
+you'll be given strong allies and a hat
+that'll help you to get stronger.</t>
   </si>
   <si>
     <t xml:space="preserve">遠くの場所へ　行きたい場合は　町にある列車や
@@ -70,8 +127,39 @@
 この広い世界の冒険を　楽しんでください。</t>
   </si>
   <si>
+    <t xml:space="preserve">Many a challenge awaits you in this grand
+world. Talking to the villagers in this town
+may provide you with some helpful information.
+&lt;br&gt;
+Quests will be marked with purple icons.
+If you find yourself lost, opening your
+map can show you the way.
+&lt;br&gt;
+To travel to faraway places, you can use a
+train station or a Zoomstone, located under
+the "Items" command.
+&lt;br&gt;
+You can find useful adventuring information
+in the "Play Guide" section using the "Misc."
+command.
+&lt;br&gt;
+Now, it is time to embark on your great
+journey. Adventure awaits!</t>
+  </si>
+  <si>
     <t xml:space="preserve">体験版では　これ以上　お礼は渡せないんだ。
 製品版で　また　その人に話しかけてくれ。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;pipipi_high&gt;Ohh, thank you! I see you've found one of
+my chosen residents! Here, this is for you!
+&lt;br&gt;
+...hang on. You're currently playing the trial
+version, so I can't give you anything else
+until you upgrade to the full version.
+&lt;br&gt;
+You'll have to speak with them again once
+you have the full version to get something.</t>
   </si>
   <si>
     <t xml:space="preserve">「宝珠を　青い炎に捧げた後も
@@ -79,11 +167,26 @@
 　今の状態が　記憶されているぞ。</t>
   </si>
   <si>
+    <t xml:space="preserve">Even after offering the jewel to the blue
+flame, your current skill and spell positions will
+stay as they are.
+&lt;br&gt;
+I've placed the stone into your bag.
+Please return here if you need my
+services again.</t>
+  </si>
+  <si>
     <t xml:space="preserve">ゴールド受け取った。
 　やりなおしの宝珠を　受け取るがいい。</t>
   </si>
   <si>
+    <t>Thank you. Please take this stone.</t>
+  </si>
+  <si>
     <t>』に　勝利した！&lt;me 58&gt;&lt;auto_bw=10000&gt;&lt;close&gt;</t>
+  </si>
+  <si>
+    <t>You emerged victorious!&lt;me 58&gt;&lt;auto_bw=10000&gt;&lt;close&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">　私の旅路の　すべてを聞きたくない？
@@ -116,6 +219,37 @@
 &lt;case_end&gt;</t>
   </si>
   <si>
+    <t xml:space="preserve">By the way, is there something you wanted to
+ask me about my journey? Where should
+I begin?
+&lt;select 1&gt;
+After escaping the Time Prison?
+Ethene Kingdom?
+Old Gran Zedora Kingdom?
+Ask about the time traveling curse.
+Future Mereade
+Ask about the cat.
+Cancel
+&lt;select_end&gt;
+&lt;case 1&gt;
+&lt;break&gt;
+&lt;case 2&gt;
+&lt;break&gt;
+&lt;case 3&gt;
+&lt;break&gt;
+&lt;case 4&gt;
+&lt;break&gt;
+&lt;case 5&gt;
+&lt;break&gt;
+&lt;case 6&gt;
+&lt;break&gt;
+&lt;case 7&gt;
+&lt;break&gt;
+&lt;case_cancel&gt;
+&lt;break&gt;
+&lt;case_end&gt;</t>
+  </si>
+  <si>
     <t xml:space="preserve">　私の旅路の　すべてを聞きたくない？
 　何から　話してあげましょうか？
 &lt;select 2&gt;
@@ -146,6 +280,37 @@
 &lt;case_end&gt;</t>
   </si>
   <si>
+    <t xml:space="preserve">By the way, is there something you wanted to
+ask me about my journey? Where should
+I begin?
+&lt;select 2&gt;
+After escaping the Time Prison?
+Ethene Kingdom?
+Old Gran Zedora Kingdom?
+Ask about the time traveling curse.
+Future Mereade
+Ask about the cat.
+Cancel
+&lt;select_end&gt;
+&lt;case 1&gt;
+&lt;break&gt;
+&lt;case 2&gt;
+&lt;break&gt;
+&lt;case 3&gt;
+&lt;break&gt;
+&lt;case 4&gt;
+&lt;break&gt;
+&lt;case 5&gt;
+&lt;break&gt;
+&lt;case 6&gt;
+&lt;break&gt;
+&lt;case 7&gt;
+&lt;break&gt;
+&lt;case_cancel&gt;
+&lt;break&gt;
+&lt;case_end&gt;</t>
+  </si>
+  <si>
     <t xml:space="preserve">　私の旅路の　すべてを聞きたくない？
 　何から　話してあげましょうか？
 &lt;select 3&gt;
@@ -176,6 +341,37 @@
 &lt;case_end&gt;</t>
   </si>
   <si>
+    <t xml:space="preserve">By the way, is there something you wanted to
+ask me about my journey? Where should
+I begin?
+&lt;select 3&gt;
+After escaping the Time Prison?
+Ethene Kingdom?
+Old Gran Zedora Kingdom?
+Ask about the time traveling curse.
+Future Mereade
+Ask about the cat.
+Cancel
+&lt;select_end&gt;
+&lt;case 1&gt;
+&lt;break&gt;
+&lt;case 2&gt;
+&lt;break&gt;
+&lt;case 3&gt;
+&lt;break&gt;
+&lt;case 4&gt;
+&lt;break&gt;
+&lt;case 5&gt;
+&lt;break&gt;
+&lt;case 6&gt;
+&lt;break&gt;
+&lt;case 7&gt;
+&lt;break&gt;
+&lt;case_cancel&gt;
+&lt;break&gt;
+&lt;case_end&gt;</t>
+  </si>
+  <si>
     <t xml:space="preserve">　私の旅路の　すべてを聞きたくない？
 　何から　話してあげましょうか？
 &lt;select 4&gt;
@@ -206,6 +402,37 @@
 &lt;case_end&gt;</t>
   </si>
   <si>
+    <t xml:space="preserve">By the way, is there something you wanted to
+ask me about my journey? Where should
+I begin?
+&lt;select 4&gt;
+After escaping the Time Prison?
+Ethene Kingdom?
+Old Gran Zedora Kingdom?
+Ask about the time traveling curse.
+Future Mereade
+Ask about the cat.
+Cancel
+&lt;select_end&gt;
+&lt;case 1&gt;
+&lt;break&gt;
+&lt;case 2&gt;
+&lt;break&gt;
+&lt;case 3&gt;
+&lt;break&gt;
+&lt;case 4&gt;
+&lt;break&gt;
+&lt;case 5&gt;
+&lt;break&gt;
+&lt;case 6&gt;
+&lt;break&gt;
+&lt;case 7&gt;
+&lt;break&gt;
+&lt;case_cancel&gt;
+&lt;break&gt;
+&lt;case_end&gt;</t>
+  </si>
+  <si>
     <t xml:space="preserve">　私の旅路の　すべてを聞きたくない？
 　何から　話してあげましょうか？
 &lt;select 5&gt;
@@ -236,6 +463,37 @@
 &lt;case_end&gt;</t>
   </si>
   <si>
+    <t xml:space="preserve">By the way, is there something you wanted to
+ask me about my journey? Where should
+I begin?
+&lt;select 5&gt;
+After escaping the Time Prison?
+Ethene Kingdom?
+Old Gran Zedora Kingdom?
+Ask about the time traveling curse.
+Future Mereade
+Ask about the cat.
+Cancel
+&lt;select_end&gt;
+&lt;case 1&gt;
+&lt;break&gt;
+&lt;case 2&gt;
+&lt;break&gt;
+&lt;case 3&gt;
+&lt;break&gt;
+&lt;case 4&gt;
+&lt;break&gt;
+&lt;case 5&gt;
+&lt;break&gt;
+&lt;case 6&gt;
+&lt;break&gt;
+&lt;case 7&gt;
+&lt;break&gt;
+&lt;case_cancel&gt;
+&lt;break&gt;
+&lt;case_end&gt;</t>
+  </si>
+  <si>
     <t xml:space="preserve">　私の旅路の　すべてを聞きたくない？
 　何から　話してあげましょうか？
 &lt;select 6&gt;
@@ -266,6 +524,37 @@
 &lt;case_end&gt;</t>
   </si>
   <si>
+    <t xml:space="preserve">By the way, is there something you wanted to
+ask me about my journey? Where should
+I begin?
+&lt;select 6&gt;
+After escaping the Time Prison?
+Ethene Kingdom?
+Old Gran Zedora Kingdom?
+Ask about the time traveling curse.
+Future Mereade
+Ask about the cat.
+Cancel
+&lt;select_end&gt;
+&lt;case 1&gt;
+&lt;break&gt;
+&lt;case 2&gt;
+&lt;break&gt;
+&lt;case 3&gt;
+&lt;break&gt;
+&lt;case 4&gt;
+&lt;break&gt;
+&lt;case 5&gt;
+&lt;break&gt;
+&lt;case 6&gt;
+&lt;break&gt;
+&lt;case 7&gt;
+&lt;break&gt;
+&lt;case_cancel&gt;
+&lt;break&gt;
+&lt;case_end&gt;</t>
+  </si>
+  <si>
     <t xml:space="preserve">　ぼくの指示が　下手だったみたいだね。
 　もう一度　一緒に　がんばってくれる？
 &lt;br&gt;
@@ -273,32 +562,75 @@
 　聖なる織り機の前に　座ってね。</t>
   </si>
   <si>
+    <t xml:space="preserve">Agh, I'm sorry, I'm sorry! I should've been
+better at giving instructions. Do you want
+to try one more time?
+&lt;br&gt;
+Whenever you're ready, please sit in front
+of the loom again.</t>
+  </si>
+  <si>
     <t xml:space="preserve">ボタンを　押してみますか？
 あと７日で　獲得できるようになります。&lt;yesno&gt;&lt;close&gt;</t>
   </si>
   <si>
+    <t xml:space="preserve">You won't receive any Golden Treasure since
+you've explored already. Press the button
+anyways? You can explore again in 7 days.&lt;yesno&gt;&lt;close&gt;</t>
+  </si>
+  <si>
     <t xml:space="preserve">ボタンを　押してみますか？
 あと６日で　獲得できるようになります。&lt;yesno&gt;&lt;close&gt;</t>
   </si>
   <si>
+    <t xml:space="preserve">You won't receive any Golden Treasure since
+you've explored already. Press the button
+anyways? You can explore again in 6 days.&lt;yesno&gt;&lt;close&gt;</t>
+  </si>
+  <si>
     <t xml:space="preserve">ボタンを　押してみますか？
 あと５日で　獲得できるようになります。&lt;yesno&gt;&lt;close&gt;</t>
   </si>
   <si>
+    <t xml:space="preserve">You won't receive any Golden Treasure since
+you've explored already. Press the button
+anyways? You can explore again in 5 days.&lt;yesno&gt;&lt;close&gt;</t>
+  </si>
+  <si>
     <t xml:space="preserve">ボタンを　押してみますか？
 あと４日で　獲得できるようになります。&lt;yesno&gt;&lt;close&gt;</t>
   </si>
   <si>
+    <t xml:space="preserve">You won't receive any Golden Treasure since
+you've explored already. Press the button
+anyways? You can explore again in 4 days.&lt;yesno&gt;&lt;close&gt;</t>
+  </si>
+  <si>
     <t xml:space="preserve">ボタンを　押してみますか？
 あと３日で　獲得できるようになります。&lt;yesno&gt;&lt;close&gt;</t>
   </si>
   <si>
+    <t xml:space="preserve">You won't receive any Golden Treasure since
+you've explored already. Press the button
+anyways? You can explore again in 3 days.&lt;yesno&gt;&lt;close&gt;</t>
+  </si>
+  <si>
     <t xml:space="preserve">ボタンを　押してみますか？
 あと２日で　獲得できるようになります。&lt;yesno&gt;&lt;close&gt;</t>
   </si>
   <si>
+    <t xml:space="preserve">You won't receive any Golden Treasure since
+you've explored already. Press the button
+anyways? You can explore again in 2 days.&lt;yesno&gt;&lt;close&gt;</t>
+  </si>
+  <si>
     <t xml:space="preserve">ボタンを　押してみますか？
 あと１日で　獲得できるようになります。&lt;yesno&gt;&lt;close&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You won't receive any Golden Treasure since
+you've explored already. Press the button
+anyways? You can explore again in 1 day.&lt;yesno&gt;&lt;close&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">　感じるぞ！　キミから　濃厚にただよう
@@ -307,6 +639,14 @@
 「キミに　戦いを挑もう！ 
 　ワガハイ考案の　クイズバトルという戦いを。
 　この挑戦　受けてくれるね？&lt;yesno&gt;&lt;break&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I see... I can feel it! I can even smell it
+on you! The makings of "the best"...
+&lt;br&gt;
+I challenge you to a battle: a quiz of my
+own design! Do you accept my challenge?&lt;yesno&gt;&lt;break&gt;
+</t>
   </si>
   <si>
     <t xml:space="preserve">　でも　ひとつ　忠告です。くれぐれも
@@ -329,6 +669,25 @@
 &lt;case_end&gt;</t>
   </si>
   <si>
+    <t xml:space="preserve">Hey! But one word of advice.
+Don't be influenced by Papilma's mouth. We
+are a customer service firm, so be polite
+&lt;br&gt;
+when dealing with clients. Okay?
+&lt;select_nc&gt;
+I understand!
+I got it.
+I'll be careful.
+&lt;select_end&gt;
+&lt;case 1&gt;
+&lt;break&gt;
+&lt;case 2&gt;
+&lt;break&gt;
+&lt;case 3&gt;
+&lt;break&gt;
+&lt;case_end&gt;</t>
+  </si>
+  <si>
     <t xml:space="preserve">　今　ボクが読んだ辺りを　探して
 　写真を　撮ってきてほしいんだ。
 &lt;br&gt;
@@ -337,6 +696,14 @@
 　戻ってきてくれないかな？　よろしく頼むよ。</t>
   </si>
   <si>
+    <t xml:space="preserve">I'd like you to head over to the area I just
+read about and take a photograph.
+&lt;br&gt;
+If you manage to take a good enough photo,
+I'm sure you can find something important.
+Could you please bring one to me?</t>
+  </si>
+  <si>
     <t xml:space="preserve">　神聖秘文の答えが　わかったのかな。
 　答えがわかったなら　ボクにも教えてくれない？
 &lt;br&gt;
@@ -349,11 +716,32 @@
 　本当に　神聖秘文を唱えるってことで　いい？&lt;yesno&gt;&lt;break&gt;</t>
   </si>
   <si>
+    <t xml:space="preserve">Could it be that you've figured out the answer
+to the sacred text? If you do, could you
+please tell me as well?
+&lt;br&gt;
+However, once you tell me, that's it. You only
+get one answer. After that, you can't attempt
+solving another sacred text for some time.
+&lt;br&gt;
+Also, if you fail to answer within the time
+limit, the investigation will be considered
+failed. Please keep that in mind. Well?&lt;yesno&gt;&lt;break&gt;</t>
+  </si>
+  <si>
     <t xml:space="preserve">すでに　解き明かしています。
 リプレイとなりますが　ふたたび　挑戦しますか？&lt;yesno&gt;&lt;break&gt;</t>
   </si>
   <si>
+    <t xml:space="preserve">You've already solved this sacred text.
+Are you all right with doing it again?&lt;yesno&gt;&lt;break&gt;</t>
+  </si>
+  <si>
     <t>クリアしました！&lt;update_quedate&gt;&lt;open_irai&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Success! The quest has been transgressed
+with finesse!&lt;update_quedate&gt;&lt;open_irai&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">クリアしました！
@@ -364,28 +752,57 @@
 　光の神殿へ　飛竜に乗って　行きましょう。</t>
   </si>
   <si>
+    <t xml:space="preserve">Let's make our way to the Temple of Light,
+the place you were given a chance at life
+once more.</t>
+  </si>
+  <si>
     <t xml:space="preserve">行くために
 一度　元の世界へ戻りますか？&lt;yesno&gt;&lt;close&gt;</t>
   </si>
   <si>
+    <t xml:space="preserve">Return to Astoltia so you can head to the
+Memory Spot?&lt;yesno&gt;&lt;close&gt;</t>
+  </si>
+  <si>
     <t xml:space="preserve">&lt;pipipi_off&gt;&lt;speed=0&gt;第１問
 答えを</t>
   </si>
   <si>
+    <t xml:space="preserve">&lt;pipipi_off&gt;&lt;speed=0&gt;Is this your final answer to the
+first question?&lt;yesno&gt;&lt;break&gt;</t>
+  </si>
+  <si>
     <t xml:space="preserve">&lt;pipipi_off&gt;&lt;speed=0&gt;第２問
 答えを</t>
   </si>
   <si>
+    <t xml:space="preserve">&lt;pipipi_off&gt;&lt;speed=0&gt;Is this your final answer to the
+second question?&lt;yesno&gt;&lt;break&gt;</t>
+  </si>
+  <si>
     <t xml:space="preserve">&lt;pipipi_off&gt;&lt;speed=0&gt;第３問
 答えを</t>
   </si>
   <si>
+    <t xml:space="preserve">&lt;pipipi_off&gt;&lt;speed=0&gt;Is this your final answer to the
+third question?&lt;yesno&gt;&lt;break&gt;</t>
+  </si>
+  <si>
     <t xml:space="preserve">&lt;pipipi_off&gt;&lt;speed=0&gt;第４問
 答えを</t>
   </si>
   <si>
+    <t xml:space="preserve">&lt;pipipi_off&gt;&lt;speed=0&gt;Is this your final answer to the
+fourth question?&lt;yesno&gt;&lt;break&gt;</t>
+  </si>
+  <si>
     <t xml:space="preserve">&lt;pipipi_off&gt;&lt;speed=0&gt;第５問
 答えを</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;pipipi_off&gt;&lt;speed=0&gt;Is this your final answer to the
+fifth question?&lt;yesno&gt;&lt;break&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">「五・七・五の それぞれの頭の２文字……
@@ -393,13 +810,30 @@
 　カミハルムイと　呼ばれるようになったのです。</t>
   </si>
   <si>
+    <t xml:space="preserve">Three words taken from this verseー"divine",
+"spring", and "idly"ーcan be said "kami",
+"haru", and "mui". That is how this city came
+&lt;br&gt;
+to be called Kamiharmui.</t>
+  </si>
+  <si>
     <t xml:space="preserve">&lt;icon_exc&gt;「なるほど　わかりましたぞ！
 　キヨクサは　ギョクサ……
 　すなわし　王座を示しておるのですな？</t>
   </si>
   <si>
+    <t xml:space="preserve">&lt;icon_exc&gt;I see, I understand now! "Thrown" is
+"throne"... So it that what it's showing,
+then?</t>
+  </si>
+  <si>
     <t xml:space="preserve">「神代過ぎ～　春の桜よ　無為に咲く～
 　清き風吹き　草木は芽吹く～。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Past ages divine, the spring blossoms bloom,
+waiting idly by... Pure winds blow and trees
+grown, budding green as the breeze is thrown."</t>
   </si>
   <si>
     <t xml:space="preserve">「さて　上の句の神　春　無為　と同様に
@@ -407,8 +841,17 @@
 　なんという言葉が　浮かんできますかな。</t>
   </si>
   <si>
+    <t xml:space="preserve">In regards to the second part of the song,
+the very last word is something you may
+want to pay attention to...</t>
+  </si>
+  <si>
     <t xml:space="preserve">「……ふむ。
 　清…草……　キヨ　クサですな。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The word "thrown"...
+Does it make you think of anything?&lt;yesno&gt;&lt;close&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">「わしは　この言葉にこそ　手がかりがあると
@@ -416,8 +859,17 @@
 　この城の中に　あるものでしょうかな？</t>
   </si>
   <si>
+    <t xml:space="preserve">I believe a clue lies within this word
+"thrown", but what could it mean...?
+Does it exist in the castle, I wonder?&lt;yesno&gt;&lt;close&gt;</t>
+  </si>
+  <si>
     <t xml:space="preserve">　このカミハルムイ城の中に　キヨクサが指す
 　何かがあると……そう　おっしゃるのかな？</t>
+  </si>
+  <si>
+    <t xml:space="preserve">So you're saying...there's something inside
+this castle that points to the word "thrown"?&lt;yesno&gt;&lt;close&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">「ほう!　 キヨクサの答えが　わかったと! 
@@ -425,34 +877,76 @@
 　写真に撮ってきてもらえますかな？</t>
   </si>
   <si>
+    <t xml:space="preserve">Oh, ho! So you've figured it out, have you?
+Then, if it's not too much trouble, could I
+bother you to take a photo of it for me?</t>
+  </si>
+  <si>
     <t xml:space="preserve">「正しい写真を撮れば　だいじなものに入るはず。
 　それを　わしに　見せてくだされ。
 　 ……ホッホッホッ。楽しみですな。</t>
   </si>
   <si>
+    <t xml:space="preserve">&lt;close_irai&gt;
+If you manage to take the correct photo, it
+will be placed in your Key Items. Please
+show it to me then. Hohoho... I'm looking
+&lt;br&gt;
+forward to it!</t>
+  </si>
+  <si>
     <t xml:space="preserve">「謎が隠されている　神代の春の歌の下の句は
 　……清き風吹き　草木は芽吹く。
 　上2文字を読むと　キヨクサとなりますな。</t>
   </si>
   <si>
+    <t xml:space="preserve">A mystery hidden in the Song of Divine
+Spring's second part... The final word
+"thrown" seems to be the key.
+&lt;open_irai&gt;</t>
+  </si>
+  <si>
     <t xml:space="preserve">「もしかすると　キヨクサという言葉の
 　読み方を変えるなど　工夫をすれば
 　答えが　見えてくるのでしょうか。</t>
   </si>
   <si>
+    <t xml:space="preserve">Perhaps if you can think of another
+word or phrase that sounds like "thrown",
+then you can figure it out.</t>
+  </si>
+  <si>
     <t xml:space="preserve">　カミハルムイ城内にある　キヨクサの指すものを
 　写真に撮ってきてもらえますかな？</t>
   </si>
   <si>
+    <t xml:space="preserve">If you could, can you take a picture of what
+you think "thrown" means from inside the
+castle?</t>
+  </si>
+  <si>
     <t xml:space="preserve">　この城の中にあるという　キヨクサが指すものを
 　写真に　収められましたのでしょうかな？</t>
   </si>
   <si>
+    <t xml:space="preserve">Oh? Were you able to take a photo of the
+"thrown" inside the castle?</t>
+  </si>
+  <si>
     <t>「おや　この写真に写っとるのは　ニコロイ王 ？</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ah, this is a photo of King Nikoroi, isn't it?
+So this is what you believe the word "thrown"
+is referring to?&lt;yesno&gt;&lt;close&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">　わしには　ニコロイ王と　キヨクサの関係が
 　わかりかねますぞ。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What? I'm not sure I'm seeing the connection
+between King Nikoroi and "thrown" here...</t>
   </si>
   <si>
     <t xml:space="preserve">「写真は　これで正しいような気もしますが……。
@@ -460,8 +954,17 @@
 　もう一度　よくお考えいただけますかな？</t>
   </si>
   <si>
+    <t xml:space="preserve">This photo does seem correct, but... Can you
+reconsider if there really is a connection
+between King Nikoroi and "thrown"?</t>
+  </si>
+  <si>
     <t xml:space="preserve">「なんと! 　ニコロイ王が　キヨクサではないと。
 　では　ニコロイ王のほかに　写っているのは……</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What?! King Nikoroi isn't related to "thrown"?
+Then, what is...?</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;pc&gt;は　なぞの小箱を
@@ -477,17 +980,46 @@
 我を開きたくば　魔女に勝利せよ。</t>
   </si>
   <si>
+    <t xml:space="preserve">&lt;pc&gt; carefully examines
+the Mystery Box.
+&lt;br&gt;
+&lt;pc&gt; finds letters engraved
+on the back side of the box!
+&lt;br&gt;
+"To the south of the chalky castle where
+the beautiful queen sings and beyond the
+decayed fence, beckons the witch
+&lt;br&gt;
+with the blue, crystalline-skin."</t>
+  </si>
+  <si>
     <t xml:space="preserve">&lt;pc&gt;は　なぞの小箱を
 じっくり　ながめてみた。
 &lt;br&gt;
 どうやら　かかっていた術が　解けているようだ！</t>
   </si>
   <si>
+    <t xml:space="preserve">&lt;pc&gt; carefully examines
+the Mystery Box.
+&lt;br&gt;
+It seems the spell has been broken!</t>
+  </si>
+  <si>
     <t xml:space="preserve">「&lt;pc&gt;　こんにちはクポ！
 　モグのあげたコインは　お役に立ったクポ？&lt;bw_break&gt;</t>
   </si>
   <si>
+    <t xml:space="preserve">&lt;pc&gt;! Hello, kupo!
+Was the coin that I gave you useful?
+&lt;bw_break&gt;</t>
+  </si>
+  <si>
     <t xml:space="preserve">　モグに　プレゼントしてくれるクポ？&lt;yesno&gt;&lt;case 1&gt;&lt;close&gt;&lt;case 2&gt;&lt;break&gt;&lt;case_cancel&gt;&lt;break&gt;&lt;case_end&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;attr&gt;&lt;feel_happy_lv3&gt;&lt;end_attr&gt;Kupo!
+Can you give me the flower I asked for, kupo?
+&lt;yesno&gt;&lt;case 1&gt;&lt;close&gt;&lt;case 2&gt;&lt;break&gt;&lt;case_cancel&gt;&lt;break&gt;&lt;case_end&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;pc&gt;たちが　扉を開けると
@@ -495,13 +1027,27 @@
 部屋の中へ　すべりこんだ！</t>
   </si>
   <si>
+    <t xml:space="preserve">When &lt;pc&gt; opens the door,
+Chupie came flying past and slipped
+through the door!</t>
+  </si>
+  <si>
     <t xml:space="preserve">「おかえりなさい！　&lt;pc&gt;様！
 　お部屋の準備も　すっかり整っておりますよ。
 　もう　お休みになりますか？&lt;yesno&gt;&lt;break&gt;</t>
   </si>
   <si>
+    <t xml:space="preserve">Welcome back!
+Your room is ready. Would you like to
+rest now?&lt;yesno&gt;&lt;break&gt;</t>
+  </si>
+  <si>
     <t xml:space="preserve">断罪の剣の内なる世界が　これまで以上に
 大きな干渉を受けているようだ。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The path forward is blocked by an obtrusion
+even larger than before.</t>
   </si>
   <si>
     <t xml:space="preserve">「そっから　『キャラの場所』ってのを選べば
@@ -513,17 +1059,65 @@
 　アバさまは　本当に　怖いっぺ。</t>
   </si>
   <si>
+    <t xml:space="preserve">&lt;attr&gt;&lt;feel_happy_lv3&gt;&lt;end_attr&gt;Huh? Are ya goin' to Abba's to apologize
+for Shinonome's mistake?!
+&lt;br&gt;
+Abba gets super scary when she's steamed.
+Hope she doesn't scold ya too much!
+&lt;br&gt;
+If ya need to find her house, open the map
+and look for her house with the shiny star
+mark.
+&lt;br&gt;
+You see "Menu Display" at the bottom of the
+map there? Open that up and select
+"NPC Location", and you can see who's where.
+&lt;br&gt;
+The other functions're useful too, so be sure
+to check 'em out.
+&lt;br&gt;
+Abba's grandson, Shini...he's so nice.
+But man, is she scary...</t>
+  </si>
+  <si>
     <t xml:space="preserve">&lt;attr&gt;&lt;feel_happy_lv3&gt;&lt;end_attr&gt;「アバさまに　しかられずに済んだだか？
 　シンイさまの　お使いで済むんなら
 　やすいもんだべ。</t>
   </si>
   <si>
+    <t xml:space="preserve">&lt;attr&gt;&lt;feel_happy_lv3&gt;&lt;end_attr&gt;So, didja manage to avoid gettin'
+scolded by Abba? You got off easy if it's
+just an errand ya need to run for Shini!
+&lt;br&gt;
+Fluffy Rice Husks can be found in the Water
+Cabin, and old man Kudai often uses Dried
+Antidotal Herbs to make tea.
+&lt;br&gt;
+If ya get lost, go ahead and open the map
+and look for the shiny star mark, 'kay?
+&lt;br&gt;
+You see "Menu Display" at the bottom of the
+map there? Open that up and select
+"NPC Location", and you can see who's where.
+&lt;br&gt;
+The other functions're useful too, so be sure
+to check 'em out.</t>
+  </si>
+  <si>
     <t xml:space="preserve">「やっと　新たな主神を見つけたのに
 　自分のやりたいことを　優先するなんて
 　どうして……。
 &lt;br&gt;
 「追いかけようと　思ったけど
 　ラキでも　ニオイをたどれなかった。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finally, after we found the new Almighty...
+He goes off and does what he wants.
+Why...?
+&lt;br&gt;
+Lycae thought about chasing after him,
+but even he couldn't track his scent.</t>
   </si>
 </sst>
 </file>
@@ -936,7 +1530,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B67"/>
+  <dimension ref="A1:C67"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="2" width="80.7109375" customWidth="1"/>
@@ -950,532 +1544,730 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="C13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="C14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="C15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="C16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="C17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="C18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="C19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="C20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+      <c r="C21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="C22" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="C23" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="C24" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="C25" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="C26" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="C27" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="C28" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="C29" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="C30" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+      <c r="C31" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>32</v>
+        <v>63</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="C32" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>33</v>
+        <v>65</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="C33" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>34</v>
+        <v>66</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="C34" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>35</v>
+        <v>68</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="C35" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>36</v>
+        <v>70</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="C36" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>37</v>
+        <v>72</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+      <c r="C37" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>38</v>
+        <v>74</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+      <c r="C38" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="C39" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>40</v>
+        <v>78</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+      <c r="C40" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+      <c r="C41" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>42</v>
+        <v>82</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+      <c r="C42" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>43</v>
+        <v>84</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+      <c r="C43" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>44</v>
+        <v>86</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+      <c r="C44" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>45</v>
+        <v>88</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+      <c r="C45" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>46</v>
+        <v>90</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+      <c r="C46" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>47</v>
+        <v>92</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+      <c r="C47" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>48</v>
+        <v>94</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+      <c r="C48" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>49</v>
+        <v>96</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+      <c r="C49" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>50</v>
+        <v>98</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+      <c r="C50" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>51</v>
+        <v>100</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="C51" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>52</v>
+        <v>102</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+      <c r="C52" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>53</v>
+        <v>104</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+      <c r="C53" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>54</v>
+        <v>106</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+      <c r="C54" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>55</v>
+        <v>108</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="C55" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>56</v>
+        <v>110</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+      <c r="C56" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>57</v>
+        <v>112</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+      <c r="C57" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>58</v>
+        <v>114</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+      <c r="C58" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>59</v>
+        <v>116</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+      <c r="C59" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>60</v>
+        <v>118</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+      <c r="C60" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>61</v>
+        <v>120</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+      <c r="C61" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>62</v>
+        <v>122</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+      <c r="C62" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>63</v>
+        <v>124</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+      <c r="C63" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>64</v>
+        <v>126</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+      <c r="C64" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>65</v>
+        <v>128</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="C65" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>66</v>
+        <v>130</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+      <c r="C66" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>67</v>
+        <v>132</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>67</v>
+        <v>133</v>
+      </c>
+      <c r="C67" t="s">
+        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>